<commit_message>
Use less entries in Data.xlsx for faster completion
</commit_message>
<xml_diff>
--- a/web-store-order-processor/devdata/Data.xlsx
+++ b/web-store-order-processor/devdata/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -64,93 +64,6 @@
   </si>
   <si>
     <t>Neil Parkinson</t>
-  </si>
-  <si>
-    <t>Vinay Goodwin</t>
-  </si>
-  <si>
-    <t>Bear Huynh</t>
-  </si>
-  <si>
-    <t>Nathanael Burch</t>
-  </si>
-  <si>
-    <t>Lewie Ridley</t>
-  </si>
-  <si>
-    <t>Sian Escobar</t>
-  </si>
-  <si>
-    <t>Sauce Labs Backpack</t>
-  </si>
-  <si>
-    <t>Kayson Morton</t>
-  </si>
-  <si>
-    <t>Hester Holding</t>
-  </si>
-  <si>
-    <t>Carrie-Ann Cobb</t>
-  </si>
-  <si>
-    <t>Alanah Barry</t>
-  </si>
-  <si>
-    <t>Lindsay Villanueva</t>
-  </si>
-  <si>
-    <t>Skyla Herbert</t>
-  </si>
-  <si>
-    <t>Aaliyah Aguirre</t>
-  </si>
-  <si>
-    <t>Reema Oconnell</t>
-  </si>
-  <si>
-    <t>Camilla Griffin</t>
-  </si>
-  <si>
-    <t>Sauce Labs Bike Light</t>
-  </si>
-  <si>
-    <t>Misha Warren</t>
-  </si>
-  <si>
-    <t>Amalia Hampton</t>
-  </si>
-  <si>
-    <t>Ahmet Ford</t>
-  </si>
-  <si>
-    <t>Iosif Woods</t>
-  </si>
-  <si>
-    <t>Hiba Swan</t>
-  </si>
-  <si>
-    <t>Elif Lees</t>
-  </si>
-  <si>
-    <t>Lenny Rasmussen</t>
-  </si>
-  <si>
-    <t>Jada Hicks</t>
-  </si>
-  <si>
-    <t>Johan Ingram</t>
-  </si>
-  <si>
-    <t>Ayush Sampson</t>
-  </si>
-  <si>
-    <t>Jaxson Whitney</t>
-  </si>
-  <si>
-    <t>Princess Townsend</t>
-  </si>
-  <si>
-    <t>Brandan Dillon</t>
   </si>
 </sst>
 </file>
@@ -771,15 +684,9 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="2">
-        <v>3061.0</v>
-      </c>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -805,15 +712,9 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="2">
-        <v>2032.0</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -839,15 +740,9 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1827.0</v>
-      </c>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -873,15 +768,9 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2">
-        <v>4677.0</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -907,15 +796,9 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="2">
-        <v>3475.0</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -941,15 +824,9 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2">
-        <v>2870.0</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -975,15 +852,9 @@
       <c r="Z16" s="2"/>
     </row>
     <row r="17">
-      <c r="A17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="2">
-        <v>2168.0</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1009,15 +880,9 @@
       <c r="Z17" s="2"/>
     </row>
     <row r="18">
-      <c r="A18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="2">
-        <v>3471.0</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1043,15 +908,9 @@
       <c r="Z18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2">
-        <v>1373.0</v>
-      </c>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1077,15 +936,9 @@
       <c r="Z19" s="2"/>
     </row>
     <row r="20">
-      <c r="A20" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="2">
-        <v>2062.0</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1111,15 +964,9 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="2">
-        <v>3008.0</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1145,15 +992,9 @@
       <c r="Z21" s="2"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="2">
-        <v>2874.0</v>
-      </c>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
@@ -1179,15 +1020,9 @@
       <c r="Z22" s="2"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="2">
-        <v>3102.0</v>
-      </c>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1213,15 +1048,9 @@
       <c r="Z23" s="2"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="2">
-        <v>1644.0</v>
-      </c>
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1247,15 +1076,9 @@
       <c r="Z24" s="2"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3270.0</v>
-      </c>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1281,15 +1104,9 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>3261.0</v>
-      </c>
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
@@ -1315,15 +1132,9 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="2">
-        <v>3512.0</v>
-      </c>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -1349,15 +1160,9 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2">
-        <v>2648.0</v>
-      </c>
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1383,15 +1188,9 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="2">
-        <v>2162.0</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1417,15 +1216,9 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" s="2">
-        <v>3703.0</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -1451,15 +1244,9 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="2">
-        <v>4518.0</v>
-      </c>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -1485,15 +1272,9 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="2">
-        <v>2647.0</v>
-      </c>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -1519,15 +1300,9 @@
       <c r="Z32" s="2"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="2">
-        <v>4961.0</v>
-      </c>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -1553,15 +1328,9 @@
       <c r="Z33" s="2"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1893.0</v>
-      </c>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -1587,15 +1356,9 @@
       <c r="Z34" s="2"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="2">
-        <v>3812.0</v>
-      </c>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -1621,15 +1384,9 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="2">
-        <v>3892.0</v>
-      </c>
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -1655,15 +1412,9 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2">
-        <v>3218.0</v>
-      </c>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>

</xml_diff>